<commit_message>
read excel partially solved
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repositories\CCSmarket\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\py\my\CCSmarket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E6515A5-2546-42E5-878F-70502BA39AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C501001-361F-474B-9960-79F5044AE4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{992F3990-0C18-49CC-B48B-4DE0C96FF87B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{992F3990-0C18-49CC-B48B-4DE0C96FF87B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="4" r:id="rId2"/>
     <sheet name="NEXE" sheetId="2" r:id="rId3"/>
-    <sheet name="NEXE (2)" sheetId="3" r:id="rId4"/>
+    <sheet name="petrokemija" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="52">
   <si>
     <t>released_CO2</t>
   </si>
@@ -168,6 +168,33 @@
   </si>
   <si>
     <t>Biorafinerija Sisak</t>
+  </si>
+  <si>
+    <t>last year</t>
+  </si>
+  <si>
+    <t>company name</t>
+  </si>
+  <si>
+    <t>facility name</t>
+  </si>
+  <si>
+    <t>core_cash_flow_start</t>
+  </si>
+  <si>
+    <t>core_cash_flow_initial</t>
+  </si>
+  <si>
+    <t>core_cash_flow_change</t>
+  </si>
+  <si>
+    <t>core_cash_flow_model</t>
+  </si>
+  <si>
+    <t>for future - to analyze how core business and CO2 market interfere</t>
+  </si>
+  <si>
+    <t>last year in time series</t>
   </si>
 </sst>
 </file>
@@ -175,8 +202,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -246,11 +273,11 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -571,24 +598,24 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -623,13 +650,16 @@
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
       </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
       <c r="G2" s="4">
         <v>0</v>
       </c>
@@ -643,12 +673,15 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
@@ -664,7 +697,7 @@
         <v>270000</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G4" s="4">
         <v>2</v>
       </c>
@@ -675,11 +708,11 @@
         <v>181500</v>
       </c>
       <c r="J4" s="4">
-        <f t="shared" ref="J4:J17" si="0">J3-30000</f>
+        <f t="shared" ref="J4:J12" si="0">J3-30000</f>
         <v>240000</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G5" s="4">
         <v>3</v>
       </c>
@@ -694,7 +727,16 @@
         <v>210000</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
       <c r="G6" s="4">
         <v>4</v>
       </c>
@@ -709,7 +751,7 @@
         <v>180000</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G7" s="4">
         <v>5</v>
       </c>
@@ -724,7 +766,7 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -750,7 +792,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -774,7 +816,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -798,7 +840,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -823,7 +865,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -847,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G13" s="4">
         <v>11</v>
       </c>
@@ -861,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -884,7 +926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -907,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -930,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -953,7 +995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G18" s="4">
         <v>16</v>
       </c>
@@ -967,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -990,7 +1032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1013,7 +1055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1036,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1059,7 +1101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G23" s="4">
         <v>21</v>
       </c>
@@ -1073,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1096,7 +1138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1119,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1142,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1165,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G28" s="4">
         <v>26</v>
       </c>
@@ -1179,7 +1221,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
       <c r="G29" s="4">
         <v>27</v>
       </c>
@@ -1193,7 +1244,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
       <c r="G30" s="4">
         <v>28</v>
       </c>
@@ -1207,7 +1267,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>-0.05</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
       <c r="G31" s="4">
         <v>29</v>
       </c>
@@ -1221,7 +1290,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
       <c r="G32" s="4"/>
     </row>
   </sheetData>
@@ -1234,23 +1312,23 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -1285,49 +1363,64 @@
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
       </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
       <c r="G2" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
       </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
       <c r="G3" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G4" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G5" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
       <c r="G6" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G7" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1343,7 +1436,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1357,7 +1450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1371,7 +1464,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1386,7 +1479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1400,12 +1493,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G13" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1419,7 +1512,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1433,7 +1526,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1447,7 +1540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1461,12 +1554,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G18" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1480,7 +1573,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1494,7 +1587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1508,7 +1601,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1522,12 +1615,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G23" s="4">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1541,7 +1634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1555,7 +1648,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1569,7 +1662,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1583,30 +1676,64 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G28" s="4">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
       <c r="G29" s="4">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
       <c r="G30" s="4">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>-0.05</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
       <c r="G31" s="4">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G32" s="4">
-        <v>30</v>
-      </c>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1618,24 +1745,24 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -1661,49 +1788,40 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>37</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1713,13 +1831,10 @@
       <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1729,11 +1844,8 @@
       <c r="C9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1743,11 +1855,8 @@
       <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1758,11 +1867,8 @@
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1772,16 +1878,8 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1791,11 +1889,8 @@
       <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="E14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1805,11 +1900,8 @@
       <c r="C15" t="s">
         <v>29</v>
       </c>
-      <c r="E15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1819,11 +1911,8 @@
       <c r="C16" t="s">
         <v>30</v>
       </c>
-      <c r="E16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1833,16 +1922,8 @@
       <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="E17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1852,11 +1933,8 @@
       <c r="C19" t="s">
         <v>28</v>
       </c>
-      <c r="E19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1866,11 +1944,8 @@
       <c r="C20" t="s">
         <v>29</v>
       </c>
-      <c r="E20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1880,11 +1955,8 @@
       <c r="C21" t="s">
         <v>30</v>
       </c>
-      <c r="E21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1894,16 +1966,8 @@
       <c r="C22" t="s">
         <v>31</v>
       </c>
-      <c r="E22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1913,11 +1977,8 @@
       <c r="C24" t="s">
         <v>28</v>
       </c>
-      <c r="E24">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1927,11 +1988,8 @@
       <c r="C25" t="s">
         <v>29</v>
       </c>
-      <c r="E25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1941,11 +1999,8 @@
       <c r="C26" t="s">
         <v>30</v>
       </c>
-      <c r="E26">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1955,33 +2010,49 @@
       <c r="C27" t="s">
         <v>31</v>
       </c>
-      <c r="E27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E28">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E29">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E30">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E31">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="C30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E32">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C31" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1995,24 +2066,24 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -2038,49 +2109,64 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
         <v>40</v>
       </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>41</v>
       </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
       <c r="E3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
       <c r="E6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2096,7 +2182,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2110,7 +2196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2124,7 +2210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2139,7 +2225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2153,12 +2239,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2172,7 +2258,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2186,7 +2272,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2200,7 +2286,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2214,12 +2300,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2233,7 +2319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2247,7 +2333,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2261,7 +2347,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2275,12 +2361,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2294,7 +2380,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2308,7 +2394,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2322,7 +2408,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2336,29 +2422,62 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
       <c r="E29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1000000</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
       <c r="E30">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>-0.01</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
       <c r="E31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E32">
-        <v>30</v>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel input works (both input methods), list of industry objects initialized, simulation tryouts started
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\py\my\CCSmarket\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repositories\CCSmarket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C501001-361F-474B-9960-79F5044AE4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DBF2BB-A6B7-48C8-A598-134159BCCA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{992F3990-0C18-49CC-B48B-4DE0C96FF87B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{992F3990-0C18-49CC-B48B-4DE0C96FF87B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -597,25 +597,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED475377-F78E-40A6-A0D5-935A546E34FF}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K31" sqref="K2:K31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="21.5546875" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -650,7 +650,7 @@
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -672,8 +672,9 @@
       <c r="J2" s="4">
         <v>300000</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -696,8 +697,9 @@
         <f>J2-30000</f>
         <v>270000</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G4" s="4">
         <v>2</v>
       </c>
@@ -711,8 +713,9 @@
         <f t="shared" ref="J4:J12" si="0">J3-30000</f>
         <v>240000</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G5" s="4">
         <v>3</v>
       </c>
@@ -726,8 +729,9 @@
         <f t="shared" si="0"/>
         <v>210000</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -750,8 +754,9 @@
         <f t="shared" si="0"/>
         <v>180000</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G7" s="4">
         <v>5</v>
       </c>
@@ -765,8 +770,9 @@
         <f t="shared" si="0"/>
         <v>150000</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -789,10 +795,11 @@
         <f t="shared" si="0"/>
         <v>120000</v>
       </c>
+      <c r="K8" s="4"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -815,8 +822,9 @@
         <f t="shared" si="0"/>
         <v>90000</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -839,8 +847,9 @@
         <f t="shared" si="0"/>
         <v>60000</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -864,8 +873,9 @@
         <f t="shared" si="0"/>
         <v>30000</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -888,8 +898,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G13" s="4">
         <v>11</v>
       </c>
@@ -902,8 +913,9 @@
       <c r="J13" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -925,8 +937,9 @@
       <c r="J14" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -948,8 +961,9 @@
       <c r="J15" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -971,8 +985,9 @@
       <c r="J16" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -994,8 +1009,9 @@
       <c r="J17" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G18" s="4">
         <v>16</v>
       </c>
@@ -1008,8 +1024,9 @@
       <c r="J18" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1031,8 +1048,9 @@
       <c r="J19" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1054,8 +1072,9 @@
       <c r="J20" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1077,8 +1096,9 @@
       <c r="J21" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1100,8 +1120,9 @@
       <c r="J22" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G23" s="4">
         <v>21</v>
       </c>
@@ -1114,8 +1135,9 @@
       <c r="J23" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1137,8 +1159,9 @@
       <c r="J24" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1160,8 +1183,9 @@
       <c r="J25" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1183,8 +1207,9 @@
       <c r="J26" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1206,8 +1231,9 @@
       <c r="J27" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G28" s="4">
         <v>26</v>
       </c>
@@ -1220,8 +1246,9 @@
       <c r="J28" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1243,8 +1270,9 @@
       <c r="J29" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -1266,8 +1294,9 @@
       <c r="J30" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -1289,8 +1318,9 @@
       <c r="J31" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -1301,6 +1331,10 @@
         <v>31</v>
       </c>
       <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1315,20 +1349,20 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.88671875" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -1363,7 +1397,7 @@
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1377,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1391,17 +1425,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G4" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G5" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1415,12 +1449,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G7" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1436,7 +1470,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1450,7 +1484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1464,7 +1498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1479,7 +1513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1493,12 +1527,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G13" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1512,7 +1546,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1526,7 +1560,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1540,7 +1574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1554,12 +1588,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G18" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1573,7 +1607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1587,7 +1621,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1601,7 +1635,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1615,12 +1649,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G23" s="4">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1634,7 +1668,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1648,7 +1682,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1662,7 +1696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1676,12 +1710,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G28" s="4">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -1695,7 +1729,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -1709,7 +1743,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -1723,7 +1757,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -1748,21 +1782,21 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -1788,7 +1822,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1799,7 +1833,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1810,7 +1844,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -1821,7 +1855,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1834,7 +1868,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1845,7 +1879,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1856,7 +1890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1868,7 +1902,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1879,7 +1913,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1890,7 +1924,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1901,7 +1935,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1912,7 +1946,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1923,7 +1957,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1934,7 +1968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1945,7 +1979,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1956,7 +1990,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1967,7 +2001,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1978,7 +2012,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1989,7 +2023,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2000,7 +2034,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2011,7 +2045,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -2022,7 +2056,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -2033,7 +2067,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -2044,7 +2078,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -2069,21 +2103,21 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -2109,7 +2143,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2123,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2137,17 +2171,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2161,12 +2195,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2182,7 +2216,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2196,7 +2230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2210,7 +2244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2225,7 +2259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2239,12 +2273,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2258,7 +2292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -2272,7 +2306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2286,7 +2320,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2300,12 +2334,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -2319,7 +2353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2333,7 +2367,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2347,7 +2381,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -2361,12 +2395,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2380,7 +2414,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2394,7 +2428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2408,7 +2442,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2422,12 +2456,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>46</v>
       </c>
@@ -2441,7 +2475,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -2455,7 +2489,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -2469,7 +2503,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Excel inputs corrected, some methods and code for authomated trading started
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repositories\CCSmarket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DBF2BB-A6B7-48C8-A598-134159BCCA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAADA086-0C61-4095-8236-672F6E79658A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{992F3990-0C18-49CC-B48B-4DE0C96FF87B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{992F3990-0C18-49CC-B48B-4DE0C96FF87B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>released_CO2</t>
   </si>
   <si>
-    <t>reduced_CO2</t>
-  </si>
-  <si>
     <t>free_allowances</t>
   </si>
   <si>
@@ -101,18 +98,6 @@
     <t>released_CO2_model</t>
   </si>
   <si>
-    <t>reduced_CO2_start</t>
-  </si>
-  <si>
-    <t>reduced_CO2_initial</t>
-  </si>
-  <si>
-    <t>reduced_CO2_change</t>
-  </si>
-  <si>
-    <t>reduced_CO2_model</t>
-  </si>
-  <si>
     <t>free_allowances_start</t>
   </si>
   <si>
@@ -195,6 +180,21 @@
   </si>
   <si>
     <t>last year in time series</t>
+  </si>
+  <si>
+    <t>removed_CO2</t>
+  </si>
+  <si>
+    <t>removed_CO2_start</t>
+  </si>
+  <si>
+    <t>removed_CO2_initial</t>
+  </si>
+  <si>
+    <t>removed_CO2_change</t>
+  </si>
+  <si>
+    <t>removed_CO2_model</t>
   </si>
 </sst>
 </file>
@@ -597,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED475377-F78E-40A6-A0D5-935A546E34FF}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K31" sqref="K2:K31"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,31 +617,31 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="6"/>
       <c r="F1" s="5"/>
       <c r="G1" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="K1" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -652,13 +652,13 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -676,13 +676,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
@@ -733,13 +733,13 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G6" s="4">
         <v>4</v>
@@ -774,13 +774,13 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3">
         <v>20000000</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" s="4">
         <v>6</v>
@@ -801,13 +801,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3">
         <v>30000000</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G9" s="4">
         <v>7</v>
@@ -826,13 +826,13 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3">
         <v>5000000</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10" s="4">
         <v>8</v>
@@ -851,14 +851,14 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3">
         <f>B8-B10-B9</f>
         <v>-15000000</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11" s="4">
         <v>9</v>
@@ -877,13 +877,13 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="10">
         <v>0.08</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="4">
         <v>10</v>
@@ -917,13 +917,13 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="7">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G14" s="4">
         <v>12</v>
@@ -941,13 +941,13 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="7">
         <v>1200000</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G15" s="4">
         <v>13</v>
@@ -965,13 +965,13 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="7">
         <v>-0.1</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G16" s="4">
         <v>14</v>
@@ -989,13 +989,13 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G17" s="4">
         <v>15</v>
@@ -1028,13 +1028,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B19" s="7">
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G19" s="4">
         <v>17</v>
@@ -1052,13 +1052,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B20" s="7">
         <v>1200000</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G20" s="4">
         <v>18</v>
@@ -1076,13 +1076,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B21" s="7">
         <v>-0.1</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G21" s="4">
         <v>19</v>
@@ -1100,13 +1100,13 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G22" s="4">
         <v>20</v>
@@ -1139,13 +1139,13 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B24" s="7">
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G24" s="4">
         <v>22</v>
@@ -1163,13 +1163,13 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B25" s="8">
         <v>300000</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G25" s="4">
         <v>23</v>
@@ -1187,13 +1187,13 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B26" s="7">
         <v>-10714.25</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G26" s="4">
         <v>24</v>
@@ -1211,13 +1211,13 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G27" s="4">
         <v>25</v>
@@ -1250,13 +1250,13 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G29" s="4">
         <v>27</v>
@@ -1274,13 +1274,13 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B30" s="3">
         <v>1000000</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G30" s="4">
         <v>28</v>
@@ -1298,13 +1298,13 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B31">
         <v>-0.05</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G31" s="4">
         <v>29</v>
@@ -1322,13 +1322,13 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
@@ -1346,7 +1346,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,31 +1364,31 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="6"/>
       <c r="F1" s="5"/>
       <c r="G1" s="6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="K1" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -1399,13 +1399,13 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -1413,13 +1413,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
@@ -1437,13 +1437,13 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G6" s="4">
         <v>4</v>
@@ -1456,13 +1456,13 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3">
         <v>125000000</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" s="4">
         <v>6</v>
@@ -1472,13 +1472,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3">
         <v>40000000</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G9" s="4">
         <v>7</v>
@@ -1486,13 +1486,13 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3">
         <v>2000000</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G10" s="4">
         <v>8</v>
@@ -1500,14 +1500,14 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3">
         <f>B8-B10-B9</f>
         <v>83000000</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G11" s="4">
         <v>9</v>
@@ -1515,13 +1515,13 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="9">
         <v>0.05</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G12" s="4">
         <v>10</v>
@@ -1534,13 +1534,13 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="7">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G14" s="4">
         <v>12</v>
@@ -1548,13 +1548,13 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="7">
         <v>1200000</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G15" s="4">
         <v>13</v>
@@ -1562,13 +1562,13 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="7">
         <v>-0.1</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G16" s="4">
         <v>14</v>
@@ -1576,13 +1576,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G17" s="4">
         <v>15</v>
@@ -1595,13 +1595,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B19" s="7">
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G19" s="4">
         <v>17</v>
@@ -1609,13 +1609,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B20" s="7">
         <v>1200000</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G20" s="4">
         <v>18</v>
@@ -1623,13 +1623,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B21" s="7">
         <v>-0.1</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G21" s="4">
         <v>19</v>
@@ -1637,13 +1637,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G22" s="4">
         <v>20</v>
@@ -1656,13 +1656,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B24" s="7">
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G24" s="4">
         <v>22</v>
@@ -1670,13 +1670,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B25" s="8">
         <v>300000</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G25" s="4">
         <v>23</v>
@@ -1684,13 +1684,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B26" s="7">
         <v>-10714.25</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G26" s="4">
         <v>24</v>
@@ -1698,13 +1698,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G27" s="4">
         <v>25</v>
@@ -1717,13 +1717,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G29" s="4">
         <v>27</v>
@@ -1731,13 +1731,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B30" s="3">
         <v>1000000</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G30" s="4">
         <v>28</v>
@@ -1745,13 +1745,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B31">
         <v>-0.05</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G31" s="4">
         <v>29</v>
@@ -1759,13 +1759,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G32" s="4"/>
     </row>
@@ -1779,7 +1779,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,295 +1798,295 @@
   <sheetData>
     <row r="1" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3">
         <v>12000000</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3">
         <v>30000000</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3">
         <v>7000000</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3">
         <f>B8-B10-B9</f>
         <v>-25000000</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="10">
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>700000</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B19">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3">
         <v>150000</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B25">
         <v>250000</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B26">
         <v>-7000</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B30" s="3">
         <v>1000000</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B31">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2099,8 +2099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85341C2E-3D32-45FB-B255-18209A5FD32D}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2119,39 +2119,39 @@
   <sheetData>
     <row r="1" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2159,13 +2159,13 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -2183,13 +2183,13 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -2202,13 +2202,13 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3">
         <v>21000000</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -2218,13 +2218,13 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3">
         <v>20000000</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -2232,13 +2232,13 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3">
         <v>400000</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -2246,14 +2246,14 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="3">
         <f>B8-B10-B9</f>
         <v>600000</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11">
         <v>9</v>
@@ -2261,13 +2261,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="10">
         <v>5.5E-2</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -2280,13 +2280,13 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E14">
         <v>12</v>
@@ -2294,13 +2294,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3">
         <v>1000000</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E15">
         <v>13</v>
@@ -2308,13 +2308,13 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>0.01</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E16">
         <v>14</v>
@@ -2322,13 +2322,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E17">
         <v>15</v>
@@ -2341,13 +2341,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B19">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E19">
         <v>17</v>
@@ -2355,13 +2355,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3">
         <v>150000</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E20">
         <v>18</v>
@@ -2369,13 +2369,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E21">
         <v>19</v>
@@ -2383,13 +2383,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E22">
         <v>20</v>
@@ -2402,13 +2402,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E24">
         <v>22</v>
@@ -2416,13 +2416,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B25">
         <v>250000</v>
       </c>
       <c r="C25" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E25">
         <v>23</v>
@@ -2430,13 +2430,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B26">
         <v>-7000</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E26">
         <v>24</v>
@@ -2444,13 +2444,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E27">
         <v>25</v>
@@ -2463,13 +2463,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E29">
         <v>27</v>
@@ -2477,13 +2477,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B30" s="3">
         <v>1000000</v>
       </c>
       <c r="C30" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E30">
         <v>28</v>
@@ -2491,13 +2491,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B31">
         <v>-0.01</v>
       </c>
       <c r="C31" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E31">
         <v>29</v>
@@ -2505,13 +2505,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added trading simulation and export of all relevant properties from a list of objects (stakeholders).
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repositories\CCSmarket\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\py\my\CCSmarket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAADA086-0C61-4095-8236-672F6E79658A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECBBA09-792C-43E9-8BDF-4218EC549214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{992F3990-0C18-49CC-B48B-4DE0C96FF87B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{992F3990-0C18-49CC-B48B-4DE0C96FF87B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -597,25 +597,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED475377-F78E-40A6-A0D5-935A546E34FF}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.6640625" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -650,7 +650,7 @@
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -674,7 +674,7 @@
       </c>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -699,7 +699,7 @@
       </c>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G4" s="4">
         <v>2</v>
       </c>
@@ -715,7 +715,7 @@
       </c>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G5" s="4">
         <v>3</v>
       </c>
@@ -731,7 +731,7 @@
       </c>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -756,7 +756,7 @@
       </c>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G7" s="4">
         <v>5</v>
       </c>
@@ -772,7 +772,7 @@
       </c>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -799,7 +799,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -824,7 +824,7 @@
       </c>
       <c r="K9" s="4"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -849,7 +849,7 @@
       </c>
       <c r="K10" s="4"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -875,7 +875,7 @@
       </c>
       <c r="K11" s="4"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -900,7 +900,7 @@
       </c>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G13" s="4">
         <v>11</v>
       </c>
@@ -915,7 +915,7 @@
       </c>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -939,7 +939,7 @@
       </c>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -963,7 +963,7 @@
       </c>
       <c r="K15" s="4"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -987,7 +987,7 @@
       </c>
       <c r="K16" s="4"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="K17" s="4"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G18" s="4">
         <v>16</v>
       </c>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="K18" s="4"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1098,7 +1098,7 @@
       </c>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G23" s="4">
         <v>21</v>
       </c>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="K23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1185,7 +1185,7 @@
       </c>
       <c r="K25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1209,7 +1209,7 @@
       </c>
       <c r="K26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="G28" s="4">
         <v>26</v>
       </c>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="K29" s="4"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="K30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1345,24 +1345,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6E420BF-E4FF-40DE-8576-12E0999284D8}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="P1" s="5"/>
       <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1425,17 +1425,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G4" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G5" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1449,12 +1449,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G7" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1470,7 +1470,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1527,12 +1527,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G13" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1588,12 +1588,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G18" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -1649,12 +1649,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G23" s="4">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1710,12 +1710,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G28" s="4">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1778,25 +1778,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF94B346-FEBD-46D1-87F7-C346238E8588}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F17" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1868,7 +1868,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1935,18 +1935,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
-        <v>5.0000000000000001E-3</v>
+        <v>0.03</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2056,7 +2056,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -2099,25 +2099,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85341C2E-3D32-45FB-B255-18209A5FD32D}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="5" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2157,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2171,17 +2171,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -2195,12 +2195,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2216,7 +2216,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2273,12 +2273,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -2334,12 +2334,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2367,7 +2367,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -2381,7 +2381,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -2395,12 +2395,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -2456,12 +2456,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>44</v>
       </c>

</xml_diff>